<commit_message>
early draft of profile
</commit_message>
<xml_diff>
--- a/docs/argo-clinicalnotes.xlsx
+++ b/docs/argo-clinicalnotes.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$62</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="419">
   <si>
     <t>Path</t>
   </si>
@@ -526,7 +526,7 @@
     <t>DocumentReference.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient]]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient]]}
 </t>
   </si>
   <si>
@@ -601,7 +601,7 @@
     <t>DocumentReference.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Practitioner], CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization], CanonicalType[http://hl7.org/fhir/StructureDefinition/Device], CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner], CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization], CanonicalType[http://hl7.org/fhir/StructureDefinition/Device], CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson]]}
 </t>
   </si>
   <si>
@@ -657,7 +657,7 @@
     <t>DocumentReference.custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization]]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization]]}
 </t>
   </si>
   <si>
@@ -872,6 +872,210 @@
   </si>
   <si>
     <t>DocumentEntry.mimeType DocumentEntry.languageCode DocumentEntry.URI DocumentEntry.size DocumentEntry.hash DocumentEntry.title</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.id</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.contentType</t>
+  </si>
+  <si>
+    <t>Mime type of the content, with charset etc.</t>
+  </si>
+  <si>
+    <t>Identifies the type of the data in the attachment and allows a method to be chosen to interpret or render the data. Includes mime type parameters such as charset where appropriate.</t>
+  </si>
+  <si>
+    <t>Processors of the data need to be able to know how to interpret the data.</t>
+  </si>
+  <si>
+    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="text/plain; charset=UTF-8, image/png"/&gt;</t>
+  </si>
+  <si>
+    <t>The mime type of an attachment. Any valid mime type is allowed.</t>
+  </si>
+  <si>
+    <t>http://www.rfc-editor.org/bcp/bcp13.txt</t>
+  </si>
+  <si>
+    <t>Attachment.contentType</t>
+  </si>
+  <si>
+    <t>./mediaType, ./charset</t>
+  </si>
+  <si>
+    <t>ED.2+ED.3/RP.2+RP.3. Note conversion may be needed if old style values are being used</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.language</t>
+  </si>
+  <si>
+    <t>Human language of the content (BCP-47)</t>
+  </si>
+  <si>
+    <t>The human language of the content. The value can be any valid value according to BCP 47.</t>
+  </si>
+  <si>
+    <t>Users need to be able to choose between the languages in a set of attachments.</t>
+  </si>
+  <si>
+    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="en-AU"/&gt;</t>
+  </si>
+  <si>
+    <t>Attachment.language</t>
+  </si>
+  <si>
+    <t>./language</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base64Binary {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Data inline, base64ed</t>
+  </si>
+  <si>
+    <t>The actual data of the attachment - a sequence of bytes. In XML, represented using base64.</t>
+  </si>
+  <si>
+    <t>The base64-encoded data SHALL be expressed in the same character set as the base resource XML or JSON.</t>
+  </si>
+  <si>
+    <t>The data needs to able to be transmitted inline.</t>
+  </si>
+  <si>
+    <t>Attachment.data</t>
+  </si>
+  <si>
+    <t>./data</t>
+  </si>
+  <si>
+    <t>ED.5</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.url</t>
+  </si>
+  <si>
+    <t>Uri where the data can be found</t>
+  </si>
+  <si>
+    <t>An alternative location where the data can be accessed.</t>
+  </si>
+  <si>
+    <t>If both data and url are provided, the url SHALL point to the same content as the data contains. Urls may be relative references or may reference transient locations such as a wrapping envelope using cid: though this has ramifications for using signatures. Relative URLs are interpreted relative to the service url, like a resource reference, rather than relative to the resource itself. If a URL is provided, it SHALL resolve to actual data.</t>
+  </si>
+  <si>
+    <t>The data needs to be transmitted by reference.</t>
+  </si>
+  <si>
+    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://www.acme.com/logo-small.png"/&gt;</t>
+  </si>
+  <si>
+    <t>Attachment.url</t>
+  </si>
+  <si>
+    <t>./reference/literal</t>
+  </si>
+  <si>
+    <t>RP.1+RP.2 - if they refer to a URL (see v2.6)</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unsignedInt {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Number of bytes of content (if url provided)</t>
+  </si>
+  <si>
+    <t>The number of bytes of data that make up this attachment (before base64 encoding, if that is done).</t>
+  </si>
+  <si>
+    <t>The number of bytes is redundant if the data is provided as a base64binary, but is useful if the data is provided as a url reference.</t>
+  </si>
+  <si>
+    <t>Representing the size allows applications to determine whether they should fetch the content automatically in advance, or refuse to fetch it at all.</t>
+  </si>
+  <si>
+    <t>Attachment.size</t>
+  </si>
+  <si>
+    <t>N/A (needs data type R3 proposal)</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.hash</t>
+  </si>
+  <si>
+    <t>Hash of the data (sha-1, base64ed)</t>
+  </si>
+  <si>
+    <t>The calculated hash of the data using SHA-1. Represented using base64.</t>
+  </si>
+  <si>
+    <t>The hash is calculated on the data prior to base64 encoding, if the data is based64 encoded.</t>
+  </si>
+  <si>
+    <t>Included so that applications can verify that the contents of a location have not changed and so that a signature of the content can implicitly sign the content of an image without having to include the data in the instance or reference the url in the signature.</t>
+  </si>
+  <si>
+    <t>Attachment.hash</t>
+  </si>
+  <si>
+    <t>.integrityCheck[parent::ED/integrityCheckAlgorithm="SHA-1"]</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.title</t>
+  </si>
+  <si>
+    <t>Label to display in place of the data</t>
+  </si>
+  <si>
+    <t>A label or set of text to display in place of the data.</t>
+  </si>
+  <si>
+    <t>Applications need a label to display to a human user in place of the actual data if the data cannot be rendered or perceived by the viewer.</t>
+  </si>
+  <si>
+    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Official Corporate Logo"/&gt;</t>
+  </si>
+  <si>
+    <t>Attachment.title</t>
+  </si>
+  <si>
+    <t>./title/data</t>
+  </si>
+  <si>
+    <t>DocumentReference.content.attachment.creation</t>
+  </si>
+  <si>
+    <t>Date attachment was first created</t>
+  </si>
+  <si>
+    <t>The date that the attachment was first created.</t>
+  </si>
+  <si>
+    <t>This is often tracked as an integrity issue for use of the attachment.</t>
+  </si>
+  <si>
+    <t>Attachment.creation</t>
   </si>
   <si>
     <t>DocumentReference.content.format</t>
@@ -1253,7 +1457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN52"/>
+  <dimension ref="A1:AN62"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1262,45 +1466,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="52.18359375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="50.6328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="74.7421875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="70.85546875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="75.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="55.90625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="44.48046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="71.41015625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="52.08203125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="43.28515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="25.015625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="87.15234375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="132.66015625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="23.95703125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="82.05078125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="127.69921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2641,7 +2845,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>121</v>
       </c>
@@ -2657,7 +2861,7 @@
         <v>50</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>51</v>
@@ -2863,7 +3067,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" hidden="true">
+    <row r="15">
       <c r="A15" t="s" s="2">
         <v>140</v>
       </c>
@@ -2879,7 +3083,7 @@
         <v>50</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>40</v>
@@ -3087,7 +3291,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>163</v>
       </c>
@@ -3103,7 +3307,7 @@
         <v>50</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>40</v>
@@ -3418,7 +3622,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
         <v>187</v>
       </c>
@@ -3434,7 +3638,7 @@
         <v>42</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>40</v>
@@ -3640,7 +3844,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
         <v>205</v>
       </c>
@@ -3656,7 +3860,7 @@
         <v>50</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>40</v>
@@ -4639,7 +4843,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" hidden="true">
+    <row r="31">
       <c r="A31" t="s" s="2">
         <v>263</v>
       </c>
@@ -4655,7 +4859,7 @@
         <v>42</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>40</v>
@@ -5079,7 +5283,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
         <v>270</v>
       </c>
@@ -5095,7 +5299,7 @@
         <v>50</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>40</v>
@@ -5210,20 +5414,18 @@
         <v>40</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>277</v>
+        <v>219</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>278</v>
+        <v>220</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>40</v>
@@ -5248,13 +5450,13 @@
         <v>40</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>281</v>
+        <v>40</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>282</v>
+        <v>40</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>40</v>
@@ -5272,7 +5474,7 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>276</v>
+        <v>222</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5287,7 +5489,7 @@
         <v>40</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>40</v>
@@ -5296,23 +5498,23 @@
         <v>40</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>283</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>40</v>
@@ -5321,19 +5523,19 @@
         <v>40</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>212</v>
+        <v>96</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>285</v>
+        <v>97</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>286</v>
+        <v>225</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>287</v>
+        <v>99</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5371,34 +5573,34 @@
         <v>40</v>
       </c>
       <c r="AA37" t="s" s="2">
-        <v>40</v>
+        <v>278</v>
       </c>
       <c r="AB37" t="s" s="2">
-        <v>40</v>
+        <v>279</v>
       </c>
       <c r="AC37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD37" t="s" s="2">
-        <v>40</v>
+        <v>280</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>284</v>
+        <v>226</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>216</v>
+        <v>40</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>288</v>
+        <v>223</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>40</v>
@@ -5410,9 +5612,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5420,31 +5622,33 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F38" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>219</v>
+        <v>69</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>220</v>
+        <v>282</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="N38" t="s" s="2">
+        <v>284</v>
+      </c>
       <c r="O38" t="s" s="2">
         <v>40</v>
       </c>
@@ -5456,7 +5660,7 @@
         <v>40</v>
       </c>
       <c r="S38" t="s" s="2">
-        <v>40</v>
+        <v>285</v>
       </c>
       <c r="T38" t="s" s="2">
         <v>40</v>
@@ -5468,13 +5672,13 @@
         <v>40</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>40</v>
+        <v>287</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>40</v>
@@ -5492,7 +5696,7 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>222</v>
+        <v>288</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5507,13 +5711,13 @@
         <v>40</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>223</v>
+        <v>289</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>40</v>
+        <v>290</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>40</v>
@@ -5521,18 +5725,18 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>40</v>
@@ -5541,21 +5745,21 @@
         <v>40</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>97</v>
+        <v>292</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="N39" s="2"/>
+        <v>293</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" t="s" s="2">
+        <v>294</v>
+      </c>
       <c r="O39" t="s" s="2">
         <v>40</v>
       </c>
@@ -5567,7 +5771,7 @@
         <v>40</v>
       </c>
       <c r="S39" t="s" s="2">
-        <v>40</v>
+        <v>295</v>
       </c>
       <c r="T39" t="s" s="2">
         <v>40</v>
@@ -5579,13 +5783,13 @@
         <v>40</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>40</v>
@@ -5603,13 +5807,13 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>226</v>
+        <v>296</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>40</v>
@@ -5618,7 +5822,7 @@
         <v>40</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>223</v>
+        <v>297</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>40</v>
@@ -5632,41 +5836,43 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>228</v>
+        <v>40</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>96</v>
+        <v>299</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>102</v>
+        <v>300</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>229</v>
+        <v>301</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="N40" s="2"/>
+        <v>302</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>303</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>40</v>
       </c>
@@ -5714,13 +5920,13 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>230</v>
+        <v>304</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>40</v>
@@ -5729,13 +5935,13 @@
         <v>40</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>93</v>
+        <v>305</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>40</v>
+        <v>306</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>40</v>
@@ -5743,7 +5949,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5751,7 +5957,7 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F41" t="s" s="2">
         <v>50</v>
@@ -5766,16 +5972,20 @@
         <v>51</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>293</v>
+        <v>63</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+        <v>309</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>311</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>40</v>
       </c>
@@ -5787,7 +5997,7 @@
         <v>40</v>
       </c>
       <c r="S41" t="s" s="2">
-        <v>40</v>
+        <v>312</v>
       </c>
       <c r="T41" t="s" s="2">
         <v>40</v>
@@ -5823,7 +6033,7 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
@@ -5838,13 +6048,13 @@
         <v>40</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>297</v>
+        <v>40</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>40</v>
+        <v>315</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>40</v>
@@ -5852,7 +6062,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5863,7 +6073,7 @@
         <v>41</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>40</v>
@@ -5875,18 +6085,20 @@
         <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>141</v>
+        <v>317</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="N42" s="2"/>
+        <v>320</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>321</v>
+      </c>
       <c r="O42" t="s" s="2">
         <v>40</v>
       </c>
@@ -5910,13 +6122,13 @@
         <v>40</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>158</v>
+        <v>40</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>302</v>
+        <v>40</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>303</v>
+        <v>40</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>40</v>
@@ -5934,13 +6146,13 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>298</v>
+        <v>322</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>40</v>
@@ -5949,7 +6161,7 @@
         <v>40</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>40</v>
@@ -5958,12 +6170,12 @@
         <v>40</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>305</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5986,16 +6198,20 @@
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+        <v>326</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>328</v>
+      </c>
       <c r="O43" t="s" s="2">
         <v>40</v>
       </c>
@@ -6043,7 +6259,7 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
@@ -6058,7 +6274,7 @@
         <v>40</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>40</v>
@@ -6067,12 +6283,12 @@
         <v>40</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>311</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6095,16 +6311,18 @@
         <v>51</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+      <c r="N44" t="s" s="2">
+        <v>334</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>40</v>
       </c>
@@ -6116,7 +6334,7 @@
         <v>40</v>
       </c>
       <c r="S44" t="s" s="2">
-        <v>40</v>
+        <v>335</v>
       </c>
       <c r="T44" t="s" s="2">
         <v>40</v>
@@ -6128,13 +6346,13 @@
         <v>40</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>158</v>
+        <v>40</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>315</v>
+        <v>40</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>316</v>
+        <v>40</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>40</v>
@@ -6152,7 +6370,7 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>312</v>
+        <v>336</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -6167,7 +6385,7 @@
         <v>40</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>40</v>
@@ -6176,12 +6394,12 @@
         <v>40</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>318</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>319</v>
+        <v>338</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6204,19 +6422,17 @@
         <v>51</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>320</v>
+        <v>339</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>322</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="M45" s="2"/>
       <c r="N45" t="s" s="2">
-        <v>323</v>
+        <v>341</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>40</v>
@@ -6241,13 +6457,13 @@
         <v>40</v>
       </c>
       <c r="W45" t="s" s="2">
-        <v>158</v>
+        <v>40</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>324</v>
+        <v>40</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="Z45" t="s" s="2">
         <v>40</v>
@@ -6265,7 +6481,7 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>319</v>
+        <v>342</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6280,7 +6496,7 @@
         <v>40</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>40</v>
@@ -6289,12 +6505,12 @@
         <v>40</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>326</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>327</v>
+        <v>343</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6317,15 +6533,17 @@
         <v>51</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M46" s="2"/>
+        <v>346</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>347</v>
+      </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>40</v>
@@ -6350,13 +6568,13 @@
         <v>40</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>40</v>
+        <v>348</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>40</v>
+        <v>349</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>40</v>
@@ -6374,7 +6592,7 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>327</v>
+        <v>343</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6389,7 +6607,7 @@
         <v>40</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>167</v>
+        <v>266</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>40</v>
@@ -6398,12 +6616,12 @@
         <v>40</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>331</v>
+        <v>350</v>
       </c>
     </row>
-    <row r="47" hidden="true">
+    <row r="47">
       <c r="A47" t="s" s="2">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6411,13 +6629,13 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>40</v>
@@ -6429,13 +6647,13 @@
         <v>212</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>333</v>
+        <v>352</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>334</v>
+        <v>353</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>335</v>
+        <v>354</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -6485,13 +6703,13 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>40</v>
@@ -6500,7 +6718,7 @@
         <v>216</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>336</v>
+        <v>355</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>40</v>
@@ -6509,12 +6727,12 @@
         <v>40</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>337</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>338</v>
+        <v>356</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6623,7 +6841,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>339</v>
+        <v>357</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6734,7 +6952,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>340</v>
+        <v>358</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6845,7 +7063,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6853,7 +7071,7 @@
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F51" t="s" s="2">
         <v>50</v>
@@ -6868,17 +7086,15 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>106</v>
+        <v>360</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>342</v>
+        <v>361</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>344</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>40</v>
@@ -6927,7 +7143,7 @@
         <v>40</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -6942,10 +7158,10 @@
         <v>40</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>345</v>
+        <v>363</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>40</v>
+        <v>364</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>40</v>
@@ -6956,7 +7172,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>346</v>
+        <v>365</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6967,7 +7183,7 @@
         <v>41</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>40</v>
@@ -6979,16 +7195,16 @@
         <v>51</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>347</v>
+        <v>141</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>348</v>
+        <v>366</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>349</v>
+        <v>367</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>350</v>
+        <v>368</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7014,13 +7230,13 @@
         <v>40</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>40</v>
+        <v>158</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>40</v>
+        <v>369</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>40</v>
+        <v>370</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>40</v>
@@ -7038,13 +7254,13 @@
         <v>40</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>346</v>
+        <v>365</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>40</v>
@@ -7053,7 +7269,7 @@
         <v>40</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>40</v>
@@ -7062,11 +7278,1115 @@
         <v>40</v>
       </c>
       <c r="AM52" t="s" s="2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="O55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="56" hidden="true">
+      <c r="A56" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F56" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P56" s="2"/>
+      <c r="Q56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM56" t="s" s="2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="57" hidden="true">
+      <c r="A57" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F57" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="N57" s="2"/>
+      <c r="O57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P57" s="2"/>
+      <c r="Q57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM57" t="s" s="2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="58" hidden="true">
+      <c r="A58" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F58" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J58" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P58" s="2"/>
+      <c r="Q58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE58" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AF58" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG58" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ58" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AK58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM58" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" hidden="true">
+      <c r="A59" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F59" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J59" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="K59" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="N59" s="2"/>
+      <c r="O59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P59" s="2"/>
+      <c r="Q59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE59" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AF59" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG59" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ59" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AK59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM59" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" hidden="true">
+      <c r="A60" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F60" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H60" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="I60" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J60" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="K60" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="N60" s="2"/>
+      <c r="O60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P60" s="2"/>
+      <c r="Q60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE60" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM60" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" hidden="true">
+      <c r="A61" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F61" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I61" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J61" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="K61" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="N61" s="2"/>
+      <c r="O61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P61" s="2"/>
+      <c r="Q61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM61" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F62" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="N62" s="2"/>
+      <c r="O62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM62" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM52">
+  <autoFilter ref="A1:AM62">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7076,7 +8396,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI51">
+  <conditionalFormatting sqref="A2:AI61">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
show how to add US Core DR
</commit_message>
<xml_diff>
--- a/docs/argo-clinicalnotes.xlsx
+++ b/docs/argo-clinicalnotes.xlsx
@@ -1466,45 +1466,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="50.6328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="52.18359375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="70.85546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="74.7421875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="71.41015625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="52.08203125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="43.28515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="75.515625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="55.90625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="44.48046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="23.95703125" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="82.05078125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="127.69921875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="25.015625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="87.15234375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="132.66015625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
improved guidance on profile page
</commit_message>
<xml_diff>
--- a/docs/argo-clinicalnotes.xlsx
+++ b/docs/argo-clinicalnotes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="415">
   <si>
     <t>Path</t>
   </si>
@@ -146,10 +146,10 @@
     <t>*</t>
   </si>
   <si>
-    <t>A reference to a document</t>
-  </si>
-  <si>
-    <t>A reference to a document.</t>
+    <t>US Core DocumentReference Profile</t>
+  </si>
+  <si>
+    <t>This is a basic constraint on DocumentRefernce for use in the US Core IG.</t>
   </si>
   <si>
     <t>Usually, this is used for documents other than those defined by FHIR.</t>
@@ -410,9 +410,6 @@
     <t>required</t>
   </si>
   <si>
-    <t>The status of the document reference.</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/ValueSet/document-reference-status</t>
   </si>
   <si>
@@ -468,10 +465,7 @@
     <t>Key metadata element describing the document, used in searching/filtering.</t>
   </si>
   <si>
-    <t>preferred</t>
-  </si>
-  <si>
-    <t>Precise type of clinical document.</t>
+    <t>This is the code specifying the precise type of document</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/c80-doc-typecodes</t>
@@ -508,13 +502,7 @@
     <t>Helps humans to assess whether the document is of interest when viewing a list of documents.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>High-level kind of a clinical document at a macro level.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/c80-doc-classcodes</t>
+    <t>http://fhir.org/guides/argonaut-clinicalnotes/ValueSet/documentreference-category</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode="COMP].target[classCode="LIST", moodCode="EVN"].code</t>
@@ -1094,9 +1082,6 @@
     <t>Note that while IHE mostly issues URNs for format types, not all documents can be identified by a URI.</t>
   </si>
   <si>
-    <t>Document Format Codes.</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/ValueSet/formatcodes</t>
   </si>
   <si>
@@ -1156,6 +1141,9 @@
   </si>
   <si>
     <t>An event can further specialize the act inherent in the type, such as  where it is simply "Procedure Report" and the procedure was a "colonoscopy". If one or more event codes are included, they shall not conflict with the values inherent in the class or type elements as such a conflict would create an ambiguous situation.</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
   <si>
     <t>This list of codes represents the main clinical acts being documented.</t>
@@ -1490,7 +1478,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="71.41015625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="52.08203125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="76.98828125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -2736,7 +2724,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" hidden="true">
+    <row r="12">
       <c r="A12" t="s" s="2">
         <v>115</v>
       </c>
@@ -2749,10 +2737,10 @@
         <v>41</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>40</v>
@@ -2907,11 +2895,9 @@
       <c r="W13" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="X13" t="s" s="2">
+      <c r="X13" s="2"/>
+      <c r="Y13" t="s" s="2">
         <v>126</v>
-      </c>
-      <c r="Y13" t="s" s="2">
-        <v>127</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>40</v>
@@ -2944,21 +2930,21 @@
         <v>40</v>
       </c>
       <c r="AJ13" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="AK13" t="s" s="2">
         <v>128</v>
       </c>
-      <c r="AK13" t="s" s="2">
+      <c r="AL13" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="AL13" t="s" s="2">
+      <c r="AM13" t="s" s="2">
         <v>130</v>
-      </c>
-      <c r="AM13" t="s" s="2">
-        <v>131</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2984,13 +2970,13 @@
         <v>69</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="L14" t="s" s="2">
         <v>133</v>
       </c>
-      <c r="L14" t="s" s="2">
+      <c r="M14" t="s" s="2">
         <v>134</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>135</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -3019,49 +3005,49 @@
         <v>125</v>
       </c>
       <c r="X14" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="Y14" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="Y14" t="s" s="2">
+      <c r="Z14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE14" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="AF14" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG14" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI14" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="Z14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE14" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="AF14" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG14" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
+      <c r="AK14" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="AL14" t="s" s="2">
         <v>138</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>139</v>
       </c>
       <c r="AM14" t="s" s="2">
         <v>40</v>
@@ -3069,7 +3055,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3092,16 +3078,16 @@
         <v>51</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="L15" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -3127,74 +3113,74 @@
         <v>40</v>
       </c>
       <c r="W15" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="X15" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="Y15" t="s" s="2">
         <v>145</v>
       </c>
-      <c r="X15" t="s" s="2">
+      <c r="Z15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE15" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="AF15" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG15" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
         <v>146</v>
       </c>
-      <c r="Y15" t="s" s="2">
+      <c r="AK15" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="Z15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE15" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="AF15" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG15" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ15" t="s" s="2">
+      <c r="AL15" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="AK15" t="s" s="2">
+      <c r="AM15" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="AL15" t="s" s="2">
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="AM15" t="s" s="2">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" hidden="true">
-      <c r="A16" t="s" s="2">
-        <v>152</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>40</v>
@@ -3203,19 +3189,19 @@
         <v>51</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="L16" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="M16" t="s" s="2">
         <v>154</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="N16" t="s" s="2">
         <v>155</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>157</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>40</v>
@@ -3240,60 +3226,58 @@
         <v>40</v>
       </c>
       <c r="W16" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="X16" s="2"/>
+      <c r="Y16" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="Z16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE16" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="AF16" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG16" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="AK16" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AL16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="X16" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="Y16" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="Z16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE16" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="AF16" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG16" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ16" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="AK16" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="AL16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>162</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3316,13 +3300,13 @@
         <v>51</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -3373,36 +3357,36 @@
         <v>40</v>
       </c>
       <c r="AE17" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="AF17" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG17" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH17" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI17" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ17" t="s" s="2">
+      <c r="AK17" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AL17" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AM17" t="s" s="2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
         <v>167</v>
-      </c>
-      <c r="AK17" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" hidden="true">
-      <c r="A18" t="s" s="2">
-        <v>171</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3416,7 +3400,7 @@
         <v>50</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>40</v>
@@ -3425,16 +3409,16 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3484,7 +3468,7 @@
         <v>40</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>41</v>
@@ -3499,21 +3483,21 @@
         <v>40</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3536,16 +3520,16 @@
         <v>51</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3595,7 +3579,7 @@
         <v>40</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>50</v>
@@ -3610,21 +3594,21 @@
         <v>40</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3647,16 +3631,16 @@
         <v>51</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3706,7 +3690,7 @@
         <v>40</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
@@ -3721,21 +3705,21 @@
         <v>40</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3758,16 +3742,16 @@
         <v>51</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3817,7 +3801,7 @@
         <v>40</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>41</v>
@@ -3832,21 +3816,21 @@
         <v>40</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3869,16 +3853,16 @@
         <v>51</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -3928,7 +3912,7 @@
         <v>40</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>41</v>
@@ -3943,7 +3927,7 @@
         <v>40</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>40</v>
@@ -3957,7 +3941,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3980,16 +3964,16 @@
         <v>51</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -4039,7 +4023,7 @@
         <v>40</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
@@ -4051,10 +4035,10 @@
         <v>40</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>40</v>
@@ -4068,7 +4052,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4091,13 +4075,13 @@
         <v>40</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -4148,7 +4132,7 @@
         <v>40</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -4163,7 +4147,7 @@
         <v>40</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>40</v>
@@ -4177,7 +4161,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4206,7 +4190,7 @@
         <v>97</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M25" t="s" s="2">
         <v>99</v>
@@ -4259,7 +4243,7 @@
         <v>40</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>41</v>
@@ -4274,7 +4258,7 @@
         <v>40</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>40</v>
@@ -4288,11 +4272,11 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -4317,7 +4301,7 @@
         <v>102</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M26" t="s" s="2">
         <v>99</v>
@@ -4370,7 +4354,7 @@
         <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>41</v>
@@ -4399,7 +4383,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4425,13 +4409,13 @@
         <v>69</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4460,10 +4444,10 @@
         <v>125</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>40</v>
@@ -4481,7 +4465,7 @@
         <v>40</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>50</v>
@@ -4496,7 +4480,7 @@
         <v>40</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>40</v>
@@ -4505,12 +4489,12 @@
         <v>40</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4533,13 +4517,13 @@
         <v>51</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4590,23 +4574,23 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="AF28" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG28" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="AF28" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG28" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH28" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI28" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ28" t="s" s="2">
-        <v>243</v>
-      </c>
       <c r="AK28" t="s" s="2">
         <v>40</v>
       </c>
@@ -4614,12 +4598,12 @@
         <v>40</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4642,19 +4626,19 @@
         <v>51</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>40</v>
@@ -4703,7 +4687,7 @@
         <v>40</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
@@ -4718,21 +4702,21 @@
         <v>40</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4755,19 +4739,19 @@
         <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>40</v>
@@ -4795,10 +4779,10 @@
         <v>73</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>40</v>
@@ -4816,7 +4800,7 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -4831,21 +4815,21 @@
         <v>40</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4856,7 +4840,7 @@
         <v>50</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>51</v>
@@ -4868,13 +4852,13 @@
         <v>51</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4925,7 +4909,7 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>50</v>
@@ -4937,10 +4921,10 @@
         <v>40</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>40</v>
@@ -4954,7 +4938,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4977,13 +4961,13 @@
         <v>40</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5034,7 +5018,7 @@
         <v>40</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
@@ -5049,7 +5033,7 @@
         <v>40</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>40</v>
@@ -5063,7 +5047,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5092,7 +5076,7 @@
         <v>97</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>99</v>
@@ -5145,7 +5129,7 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
@@ -5160,7 +5144,7 @@
         <v>40</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>40</v>
@@ -5174,11 +5158,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5203,7 +5187,7 @@
         <v>102</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>99</v>
@@ -5256,7 +5240,7 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5285,7 +5269,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5308,13 +5292,13 @@
         <v>51</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5365,36 +5349,36 @@
         <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL35" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="AF35" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG35" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>274</v>
-      </c>
       <c r="AM35" t="s" s="2">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5417,13 +5401,13 @@
         <v>40</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5474,7 +5458,7 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5489,7 +5473,7 @@
         <v>40</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>40</v>
@@ -5503,7 +5487,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5532,7 +5516,7 @@
         <v>97</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M37" t="s" s="2">
         <v>99</v>
@@ -5573,19 +5557,19 @@
         <v>40</v>
       </c>
       <c r="AA37" t="s" s="2">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="AB37" t="s" s="2">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="AC37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD37" t="s" s="2">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5600,7 +5584,7 @@
         <v>40</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>40</v>
@@ -5614,7 +5598,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5640,14 +5624,14 @@
         <v>69</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -5660,7 +5644,7 @@
         <v>40</v>
       </c>
       <c r="S38" t="s" s="2">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="T38" t="s" s="2">
         <v>40</v>
@@ -5675,49 +5659,49 @@
         <v>125</v>
       </c>
       <c r="X38" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="Y38" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="Z38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE38" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG38" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="Y38" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="Z38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE38" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AF38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>290</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>40</v>
@@ -5725,7 +5709,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5751,14 +5735,14 @@
         <v>69</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>40</v>
@@ -5771,7 +5755,7 @@
         <v>40</v>
       </c>
       <c r="S39" t="s" s="2">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="T39" t="s" s="2">
         <v>40</v>
@@ -5807,7 +5791,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5822,7 +5806,7 @@
         <v>40</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>40</v>
@@ -5836,7 +5820,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5859,19 +5843,19 @@
         <v>40</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="N40" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="K40" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>40</v>
@@ -5920,7 +5904,7 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -5935,21 +5919,21 @@
         <v>40</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="41" hidden="true">
+    <row r="41">
       <c r="A41" t="s" s="2">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5957,13 +5941,13 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F41" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>40</v>
@@ -5975,16 +5959,16 @@
         <v>63</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>40</v>
@@ -5997,72 +5981,72 @@
         <v>40</v>
       </c>
       <c r="S41" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="AM41" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" hidden="true">
+      <c r="A42" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="T41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="AF41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6076,7 +6060,7 @@
         <v>50</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>40</v>
@@ -6085,19 +6069,19 @@
         <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="N42" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="K42" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>40</v>
@@ -6146,7 +6130,7 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -6161,7 +6145,7 @@
         <v>40</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>40</v>
@@ -6175,7 +6159,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6198,19 +6182,19 @@
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>40</v>
@@ -6259,7 +6243,7 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
@@ -6274,7 +6258,7 @@
         <v>40</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>40</v>
@@ -6288,7 +6272,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6311,17 +6295,17 @@
         <v>51</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" t="s" s="2">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>40</v>
@@ -6334,7 +6318,7 @@
         <v>40</v>
       </c>
       <c r="S44" t="s" s="2">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="T44" t="s" s="2">
         <v>40</v>
@@ -6370,7 +6354,7 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -6385,7 +6369,7 @@
         <v>40</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>40</v>
@@ -6399,7 +6383,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6422,17 +6406,17 @@
         <v>51</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" t="s" s="2">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>40</v>
@@ -6481,7 +6465,7 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6496,7 +6480,7 @@
         <v>40</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>40</v>
@@ -6510,7 +6494,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6533,16 +6517,16 @@
         <v>51</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6568,13 +6552,11 @@
         <v>40</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="X46" t="s" s="2">
-        <v>348</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="X46" s="2"/>
       <c r="Y46" t="s" s="2">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>40</v>
@@ -6592,7 +6574,7 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6607,7 +6589,7 @@
         <v>40</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>40</v>
@@ -6616,12 +6598,12 @@
         <v>40</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6629,7 +6611,7 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F47" t="s" s="2">
         <v>50</v>
@@ -6644,16 +6626,16 @@
         <v>51</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -6703,7 +6685,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6715,10 +6697,10 @@
         <v>40</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>40</v>
@@ -6732,7 +6714,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6755,13 +6737,13 @@
         <v>40</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6812,7 +6794,7 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6827,7 +6809,7 @@
         <v>40</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>40</v>
@@ -6841,7 +6823,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6870,7 +6852,7 @@
         <v>97</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M49" t="s" s="2">
         <v>99</v>
@@ -6923,7 +6905,7 @@
         <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
@@ -6938,7 +6920,7 @@
         <v>40</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>40</v>
@@ -6952,11 +6934,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -6981,7 +6963,7 @@
         <v>102</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>99</v>
@@ -7034,7 +7016,7 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -7063,7 +7045,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7086,13 +7068,13 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7143,25 +7125,25 @@
         <v>40</v>
       </c>
       <c r="AE51" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="AF51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG51" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AK51" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AF51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG51" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ51" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>364</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>40</v>
@@ -7172,7 +7154,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7195,16 +7177,16 @@
         <v>51</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7230,13 +7212,13 @@
         <v>40</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>158</v>
+        <v>364</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>40</v>
@@ -7254,7 +7236,7 @@
         <v>40</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7269,7 +7251,7 @@
         <v>40</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>40</v>
@@ -7278,12 +7260,12 @@
         <v>40</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7306,13 +7288,13 @@
         <v>51</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7363,23 +7345,23 @@
         <v>40</v>
       </c>
       <c r="AE53" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="AF53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG53" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>377</v>
-      </c>
       <c r="AK53" t="s" s="2">
         <v>40</v>
       </c>
@@ -7387,12 +7369,12 @@
         <v>40</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7415,13 +7397,13 @@
         <v>51</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7448,13 +7430,13 @@
         <v>40</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>158</v>
+        <v>364</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>40</v>
@@ -7472,7 +7454,7 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7487,7 +7469,7 @@
         <v>40</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>40</v>
@@ -7496,12 +7478,12 @@
         <v>40</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7524,19 +7506,19 @@
         <v>51</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>40</v>
@@ -7561,13 +7543,13 @@
         <v>40</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>158</v>
+        <v>364</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>40</v>
@@ -7585,7 +7567,7 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7600,7 +7582,7 @@
         <v>40</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>40</v>
@@ -7609,12 +7591,12 @@
         <v>40</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7637,13 +7619,13 @@
         <v>51</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7694,36 +7676,36 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM56" t="s" s="2">
         <v>394</v>
-      </c>
-      <c r="AF56" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG56" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH56" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI56" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ56" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="AK56" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL56" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM56" t="s" s="2">
-        <v>398</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7746,16 +7728,16 @@
         <v>51</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -7805,7 +7787,7 @@
         <v>40</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -7817,10 +7799,10 @@
         <v>40</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>40</v>
@@ -7829,12 +7811,12 @@
         <v>40</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7857,13 +7839,13 @@
         <v>40</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7914,7 +7896,7 @@
         <v>40</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -7929,7 +7911,7 @@
         <v>40</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>40</v>
@@ -7943,7 +7925,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7972,7 +7954,7 @@
         <v>97</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M59" t="s" s="2">
         <v>99</v>
@@ -8025,7 +8007,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8040,7 +8022,7 @@
         <v>40</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>40</v>
@@ -8054,11 +8036,11 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8083,7 +8065,7 @@
         <v>102</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>99</v>
@@ -8136,7 +8118,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8165,7 +8147,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8191,13 +8173,13 @@
         <v>106</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
@@ -8247,22 +8229,22 @@
         <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH61" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI61" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>412</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>40</v>
@@ -8276,7 +8258,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8299,16 +8281,16 @@
         <v>51</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8358,7 +8340,7 @@
         <v>40</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8373,7 +8355,7 @@
         <v>40</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="AK62" t="s" s="2">
         <v>40</v>

</xml_diff>

<commit_message>
updates to DR value set
</commit_message>
<xml_diff>
--- a/docs/argo-clinicalnotes.xlsx
+++ b/docs/argo-clinicalnotes.xlsx
@@ -896,7 +896,7 @@
     <t>The mime type of an attachment. Any valid mime type is allowed.</t>
   </si>
   <si>
-    <t>http://www.rfc-editor.org/bcp/bcp13.txt</t>
+    <t>http://hl7.org/fhir/ValueSet/mimetypes</t>
   </si>
   <si>
     <t>Attachment.contentType</t>
@@ -3495,7 +3495,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
         <v>176</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>50</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>40</v>

</xml_diff>

<commit_message>
review and edits and qa
</commit_message>
<xml_diff>
--- a/docs/argo-clinicalnotes.xlsx
+++ b/docs/argo-clinicalnotes.xlsx
@@ -1454,45 +1454,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="50.6328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="49.74609375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="70.85546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="70.24609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="71.41015625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="76.98828125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="43.28515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="70.828125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="77.328125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="42.26171875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="23.95703125" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="82.05078125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="127.69921875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="23.6171875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="81.6875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="125.515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
add package-list  fixed most of the link errors and  many qa errors and warnings  updated  framework
</commit_message>
<xml_diff>
--- a/docs/argo-clinicalnotes.xlsx
+++ b/docs/argo-clinicalnotes.xlsx
@@ -1454,45 +1454,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="50.6328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="49.74609375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="70.85546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="70.24609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="71.41015625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="76.98828125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="43.28515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="70.828125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="77.328125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="42.26171875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="23.95703125" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="82.05078125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="127.69921875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="23.6171875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="81.6875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="125.515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
change canonical, update package list, history path,  to meet publishing requirements
</commit_message>
<xml_diff>
--- a/docs/argo-clinicalnotes.xlsx
+++ b/docs/argo-clinicalnotes.xlsx
@@ -502,7 +502,7 @@
     <t>Helps humans to assess whether the document is of interest when viewing a list of documents.</t>
   </si>
   <si>
-    <t>http://fhir.org/guides/argonaut-clinicalnotes/ValueSet/documentreference-category</t>
+    <t>http://fhir.org/guides/argonaut/clinicalnotes/ValueSet/documentreference-category</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode="COMP].target[classCode="LIST", moodCode="EVN"].code</t>
@@ -1478,7 +1478,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="70.828125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="77.328125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="77.2265625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>

</xml_diff>